<commit_message>
Change index scale for figures
</commit_message>
<xml_diff>
--- a/figures/fig2.xlsx
+++ b/figures/fig2.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joanna\Dropbox\Repositories\ISSP_Income-Pooling\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{005DB2C9-B097-40C8-AACF-8FFE4F17125B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225BDA62-99BC-4C50-8076-DEC504BE5998}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{8BB5332C-FFBD-4228-89AC-80112EE679CF}"/>
+    <workbookView xWindow="-30828" yWindow="-1860" windowWidth="30936" windowHeight="16896" xr2:uid="{8BB5332C-FFBD-4228-89AC-80112EE679CF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="fig2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$179</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'fig2'!$A$1:$F$89</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -68,7 +70,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -101,7 +103,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -416,21 +418,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FFD989-C578-4B84-8B1A-6542A5A3216B}">
-  <dimension ref="A1:F174"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF66AAC4-CEE8-41C4-AFD3-EB67B674149F}">
+  <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.06640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -455,2263 +453,1747 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>0.13197326000000001</v>
+        <v>0.11780450000000001</v>
       </c>
       <c r="D2" s="2">
-        <v>0.60602995000000004</v>
+        <v>0.59505940999999996</v>
       </c>
       <c r="E2" s="2">
-        <v>0.17280043</v>
+        <v>0.20383783999999999</v>
       </c>
       <c r="F2" s="2">
-        <v>8.9196349999999994E-2</v>
+        <v>8.3298250000000004E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
-        <v>0.13984426</v>
+        <v>0.13197326000000001</v>
       </c>
       <c r="D3" s="2">
-        <v>0.56597595999999994</v>
+        <v>0.60602995000000004</v>
       </c>
       <c r="E3" s="2">
-        <v>0.18455239000000001</v>
+        <v>0.17280043</v>
       </c>
       <c r="F3" s="2">
-        <v>0.1096274</v>
+        <v>8.9196349999999994E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>0.05</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
-        <v>0.11780450000000001</v>
+        <v>0.13984425</v>
       </c>
       <c r="D4" s="2">
-        <v>0.59505940999999996</v>
+        <v>0.56597595999999994</v>
       </c>
       <c r="E4" s="2">
-        <v>0.20383783999999999</v>
+        <v>0.18455239000000001</v>
       </c>
       <c r="F4" s="2">
-        <v>8.3298250000000004E-2</v>
+        <v>0.1096274</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="C5" s="2">
-        <v>0.14213105000000001</v>
+        <v>0.12322292999999999</v>
       </c>
       <c r="D5" s="2">
-        <v>0.59178783999999995</v>
+        <v>0.59031889000000004</v>
       </c>
       <c r="E5" s="2">
-        <v>0.1742745</v>
+        <v>0.20014572</v>
       </c>
       <c r="F5" s="2">
-        <v>9.1806609999999997E-2</v>
+        <v>8.6312470000000002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="C6" s="2">
-        <v>0.14760804999999999</v>
+        <v>0.14213105000000001</v>
       </c>
       <c r="D6" s="2">
-        <v>0.55542431999999997</v>
+        <v>0.59178783999999995</v>
       </c>
       <c r="E6" s="2">
-        <v>0.18553517999999999</v>
+        <v>0.1742745</v>
       </c>
       <c r="F6" s="2">
-        <v>0.11143246</v>
+        <v>9.1806609999999997E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0000000000000009</v>
       </c>
       <c r="C7" s="2">
-        <v>0.12322292999999999</v>
+        <v>0.14760804999999999</v>
       </c>
       <c r="D7" s="2">
-        <v>0.59031889000000004</v>
+        <v>0.55542431999999997</v>
       </c>
       <c r="E7" s="2">
-        <v>0.20014572</v>
+        <v>0.18553517999999999</v>
       </c>
       <c r="F7" s="2">
-        <v>8.6312470000000002E-2</v>
+        <v>0.11143246</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2">
-        <v>0.15286445000000001</v>
+        <v>0.12882621</v>
       </c>
       <c r="D8" s="2">
-        <v>0.57717531</v>
+        <v>0.58535387000000005</v>
       </c>
       <c r="E8" s="2">
-        <v>0.17557021</v>
+        <v>0.19642855000000001</v>
       </c>
       <c r="F8" s="2">
-        <v>9.439003E-2</v>
+        <v>8.9391380000000006E-2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2">
-        <v>0.15568668999999999</v>
+        <v>0.15286445000000001</v>
       </c>
       <c r="D9" s="2">
-        <v>0.54470019999999997</v>
+        <v>0.57717531</v>
       </c>
       <c r="E9" s="2">
-        <v>0.18641277000000001</v>
+        <v>0.17557021</v>
       </c>
       <c r="F9" s="2">
-        <v>0.11320034</v>
+        <v>9.439003E-2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>0.09</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2">
-        <v>0.12882621</v>
+        <v>0.15568668999999999</v>
       </c>
       <c r="D10" s="2">
-        <v>0.58535386</v>
+        <v>0.54470019999999997</v>
       </c>
       <c r="E10" s="2">
-        <v>0.19642855000000001</v>
+        <v>0.18641277000000001</v>
       </c>
       <c r="F10" s="2">
-        <v>8.9391380000000006E-2</v>
+        <v>0.11320034</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2">
-        <v>0.16417877</v>
+        <v>0.1346154</v>
       </c>
       <c r="D11" s="2">
-        <v>0.56220840999999999</v>
+        <v>0.58016345000000002</v>
       </c>
       <c r="E11" s="2">
-        <v>0.17667635000000001</v>
+        <v>0.192688</v>
       </c>
       <c r="F11" s="2">
-        <v>9.6936469999999997E-2</v>
+        <v>9.2533160000000003E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2">
-        <v>0.16408186999999999</v>
+        <v>0.16417877</v>
       </c>
       <c r="D12" s="2">
-        <v>0.53381082000000002</v>
+        <v>0.56220840999999999</v>
       </c>
       <c r="E12" s="2">
-        <v>0.18718066999999999</v>
+        <v>0.17667635000000001</v>
       </c>
       <c r="F12" s="2">
-        <v>0.11492664</v>
+        <v>9.6936469999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13">
-        <v>0.11</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2">
-        <v>0.13461539</v>
+        <v>0.16408186999999999</v>
       </c>
       <c r="D13" s="2">
-        <v>0.58016345000000002</v>
+        <v>0.53381082000000002</v>
       </c>
       <c r="E13" s="2">
-        <v>0.192688</v>
+        <v>0.18718066999999999</v>
       </c>
       <c r="F13" s="2">
-        <v>9.2533160000000003E-2</v>
+        <v>0.11492664</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B14">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2">
-        <v>0.17607573000000001</v>
+        <v>0.14059110999999999</v>
       </c>
       <c r="D14" s="2">
-        <v>0.54690667000000004</v>
+        <v>0.57474727000000003</v>
       </c>
       <c r="E14" s="2">
-        <v>0.17758217000000001</v>
+        <v>0.18892587</v>
       </c>
       <c r="F14" s="2">
-        <v>9.943544E-2</v>
+        <v>9.5735749999999994E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="C15" s="2">
-        <v>0.17279417</v>
+        <v>0.17607573000000001</v>
       </c>
       <c r="D15" s="2">
-        <v>0.52276436000000004</v>
+        <v>0.54690665999999999</v>
       </c>
       <c r="E15" s="2">
-        <v>0.18783457000000001</v>
+        <v>0.17758217000000001</v>
       </c>
       <c r="F15" s="2">
-        <v>0.1166069</v>
+        <v>9.943544E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16">
-        <v>0.13</v>
+        <v>13</v>
       </c>
       <c r="C16" s="2">
-        <v>0.14059110999999999</v>
+        <v>0.17279417</v>
       </c>
       <c r="D16" s="2">
-        <v>0.57474727000000003</v>
+        <v>0.52276436000000004</v>
       </c>
       <c r="E16" s="2">
-        <v>0.18892587</v>
+        <v>0.18783457000000001</v>
       </c>
       <c r="F16" s="2">
-        <v>9.5735749999999994E-2</v>
+        <v>0.1166069</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B17">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="C17" s="2">
-        <v>0.18855321</v>
+        <v>0.14675352999999999</v>
       </c>
       <c r="D17" s="2">
-        <v>0.53129316000000004</v>
+        <v>0.56910552000000003</v>
       </c>
       <c r="E17" s="2">
-        <v>0.17827755000000001</v>
+        <v>0.18514412</v>
       </c>
       <c r="F17" s="2">
-        <v>0.10187607999999999</v>
+        <v>9.8996829999999994E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2">
-        <v>0.18182309999999999</v>
+        <v>0.1885532</v>
       </c>
       <c r="D18" s="2">
-        <v>0.51156994</v>
+        <v>0.53129316000000004</v>
       </c>
       <c r="E18" s="2">
-        <v>0.18837033</v>
+        <v>0.17827755000000001</v>
       </c>
       <c r="F18" s="2">
-        <v>0.11823663</v>
+        <v>0.10187607999999999</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19">
-        <v>0.15</v>
+        <v>15</v>
       </c>
       <c r="C19" s="2">
-        <v>0.14675352999999999</v>
+        <v>0.18182309999999999</v>
       </c>
       <c r="D19" s="2">
-        <v>0.56910552000000003</v>
+        <v>0.51156994</v>
       </c>
       <c r="E19" s="2">
-        <v>0.18514412</v>
+        <v>0.18837033</v>
       </c>
       <c r="F19" s="2">
-        <v>9.8996829999999994E-2</v>
+        <v>0.11823663</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B20">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="C20" s="2">
-        <v>0.20160489000000001</v>
+        <v>0.15310231999999999</v>
       </c>
       <c r="D20" s="2">
-        <v>0.51539455000000001</v>
+        <v>0.56323898999999999</v>
       </c>
       <c r="E20" s="2">
-        <v>0.1787532</v>
+        <v>0.18134486</v>
       </c>
       <c r="F20" s="2">
-        <v>0.10424736</v>
+        <v>0.10231382999999999</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="C21" s="2">
-        <v>0.19116691999999999</v>
+        <v>0.20160489000000001</v>
       </c>
       <c r="D21" s="2">
-        <v>0.50023766000000003</v>
+        <v>0.51539455000000001</v>
       </c>
       <c r="E21" s="2">
-        <v>0.18878407999999999</v>
+        <v>0.1787532</v>
       </c>
       <c r="F21" s="2">
-        <v>0.11981134</v>
+        <v>0.10424736</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22">
-        <v>0.17</v>
+        <v>17</v>
       </c>
       <c r="C22" s="2">
-        <v>0.15310231999999999</v>
+        <v>0.19116691999999999</v>
       </c>
       <c r="D22" s="2">
-        <v>0.56323898999999999</v>
+        <v>0.50023766000000003</v>
       </c>
       <c r="E22" s="2">
-        <v>0.18134486</v>
+        <v>0.18878407999999999</v>
       </c>
       <c r="F22" s="2">
-        <v>0.10231382999999999</v>
+        <v>0.11981134</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B23">
-        <v>0.19</v>
+        <v>19</v>
       </c>
       <c r="C23" s="2">
-        <v>0.21522016999999999</v>
+        <v>0.15963668</v>
       </c>
       <c r="D23" s="2">
-        <v>0.49924101999999998</v>
+        <v>0.55714905000000003</v>
       </c>
       <c r="E23" s="2">
-        <v>0.17900073999999999</v>
+        <v>0.17753032999999999</v>
       </c>
       <c r="F23" s="2">
-        <v>0.10653807</v>
+        <v>0.10568394</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24">
-        <v>0.19</v>
+        <v>19</v>
       </c>
       <c r="C24" s="2">
-        <v>0.20082269999999999</v>
+        <v>0.21522016999999999</v>
       </c>
       <c r="D24" s="2">
-        <v>0.48877857000000002</v>
+        <v>0.49924101999999998</v>
       </c>
       <c r="E24" s="2">
-        <v>0.18907218000000001</v>
+        <v>0.17900073999999999</v>
       </c>
       <c r="F24" s="2">
-        <v>0.12132655000000001</v>
+        <v>0.10653807</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25">
-        <v>0.19</v>
+        <v>19</v>
       </c>
       <c r="C25" s="2">
-        <v>0.15963667000000001</v>
+        <v>0.20082270999999999</v>
       </c>
       <c r="D25" s="2">
-        <v>0.55714905000000003</v>
+        <v>0.48877855999999997</v>
       </c>
       <c r="E25" s="2">
-        <v>0.17753032999999999</v>
+        <v>0.18907218000000001</v>
       </c>
       <c r="F25" s="2">
-        <v>0.10568394</v>
+        <v>0.12132655000000001</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B26">
-        <v>0.21</v>
+        <v>21</v>
       </c>
       <c r="C26" s="2">
-        <v>0.22938394000000001</v>
+        <v>0.16635525000000001</v>
       </c>
       <c r="D26" s="2">
-        <v>0.48286614999999999</v>
+        <v>0.55083771000000004</v>
       </c>
       <c r="E26" s="2">
-        <v>0.17901288000000001</v>
+        <v>0.17370294</v>
       </c>
       <c r="F26" s="2">
-        <v>0.10873703</v>
+        <v>0.10910409</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27">
-        <v>0.21</v>
+        <v>21</v>
       </c>
       <c r="C27" s="2">
-        <v>0.21078622999999999</v>
+        <v>0.22938394000000001</v>
       </c>
       <c r="D27" s="2">
-        <v>0.47720463000000002</v>
+        <v>0.48286614</v>
       </c>
       <c r="E27" s="2">
-        <v>0.18923133</v>
+        <v>0.17901288000000001</v>
       </c>
       <c r="F27" s="2">
-        <v>0.12277781</v>
+        <v>0.10873703</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28">
-        <v>0.21</v>
+        <v>21</v>
       </c>
       <c r="C28" s="2">
-        <v>0.16635525000000001</v>
+        <v>0.21078622999999999</v>
       </c>
       <c r="D28" s="2">
-        <v>0.55083771999999998</v>
+        <v>0.47720463000000002</v>
       </c>
       <c r="E28" s="2">
-        <v>0.17370294999999999</v>
+        <v>0.18923133</v>
       </c>
       <c r="F28" s="2">
-        <v>0.10910409</v>
+        <v>0.12277781</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B29">
-        <v>0.23</v>
+        <v>23</v>
       </c>
       <c r="C29" s="2">
-        <v>0.24407654000000001</v>
+        <v>0.17325615999999999</v>
       </c>
       <c r="D29" s="2">
-        <v>0.46630670000000002</v>
+        <v>0.54430765000000003</v>
       </c>
       <c r="E29" s="2">
-        <v>0.17878361000000001</v>
+        <v>0.16986523000000001</v>
       </c>
       <c r="F29" s="2">
-        <v>0.11083316</v>
+        <v>0.11257096</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30">
-        <v>0.23</v>
+        <v>23</v>
       </c>
       <c r="C30" s="2">
-        <v>0.22105198000000001</v>
+        <v>0.24407653000000001</v>
       </c>
       <c r="D30" s="2">
-        <v>0.46552873</v>
+        <v>0.46630670000000002</v>
       </c>
       <c r="E30" s="2">
-        <v>0.18925852000000001</v>
+        <v>0.17878361000000001</v>
       </c>
       <c r="F30" s="2">
-        <v>0.12416077</v>
+        <v>0.11083316</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31">
-        <v>0.23</v>
+        <v>23</v>
       </c>
       <c r="C31" s="2">
-        <v>0.17325615999999999</v>
+        <v>0.22105198000000001</v>
       </c>
       <c r="D31" s="2">
-        <v>0.54430765000000003</v>
+        <v>0.46552873</v>
       </c>
       <c r="E31" s="2">
-        <v>0.16986523000000001</v>
+        <v>0.18925852000000001</v>
       </c>
       <c r="F31" s="2">
-        <v>0.11257096</v>
+        <v>0.12416077</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B32">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="C32" s="2">
-        <v>0.25927375000000003</v>
+        <v>0.18033697000000001</v>
       </c>
       <c r="D32" s="2">
-        <v>0.44960241000000001</v>
+        <v>0.53756219999999999</v>
       </c>
       <c r="E32" s="2">
-        <v>0.17830824000000001</v>
+        <v>0.16601984</v>
       </c>
       <c r="F32" s="2">
-        <v>0.1128156</v>
+        <v>0.11608098</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B33">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="C33" s="2">
-        <v>0.23161309999999999</v>
+        <v>0.25927375000000003</v>
       </c>
       <c r="D33" s="2">
-        <v>0.45376460000000002</v>
+        <v>0.44960241000000001</v>
       </c>
       <c r="E33" s="2">
-        <v>0.18915114999999999</v>
+        <v>0.17830824000000001</v>
       </c>
       <c r="F33" s="2">
-        <v>0.12547116</v>
+        <v>0.1128156</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="C34" s="2">
-        <v>0.18033697000000001</v>
+        <v>0.23161309999999999</v>
       </c>
       <c r="D34" s="2">
-        <v>0.53756219999999999</v>
+        <v>0.45376460000000002</v>
       </c>
       <c r="E34" s="2">
-        <v>0.16601984</v>
+        <v>0.18915114999999999</v>
       </c>
       <c r="F34" s="2">
-        <v>0.11608098</v>
+        <v>0.12547116</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B35">
-        <v>0.27</v>
+        <v>27</v>
       </c>
       <c r="C35" s="2">
-        <v>0.27494698000000001</v>
+        <v>0.18759469000000001</v>
       </c>
       <c r="D35" s="2">
-        <v>0.43279557000000002</v>
+        <v>0.53060536000000003</v>
       </c>
       <c r="E35" s="2">
-        <v>0.17758359000000001</v>
+        <v>0.16216958000000001</v>
       </c>
       <c r="F35" s="2">
-        <v>0.11467386</v>
+        <v>0.11963037</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B36">
-        <v>0.27</v>
+        <v>27</v>
       </c>
       <c r="C36" s="2">
-        <v>0.24246144</v>
+        <v>0.27494697000000001</v>
       </c>
       <c r="D36" s="2">
-        <v>0.44192675999999997</v>
+        <v>0.43279558000000001</v>
       </c>
       <c r="E36" s="2">
-        <v>0.18890697000000001</v>
+        <v>0.17758359000000001</v>
       </c>
       <c r="F36" s="2">
-        <v>0.12670482999999999</v>
+        <v>0.11467386</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B37">
-        <v>0.27</v>
+        <v>27</v>
       </c>
       <c r="C37" s="2">
-        <v>0.18759469000000001</v>
+        <v>0.24246143000000001</v>
       </c>
       <c r="D37" s="2">
-        <v>0.53060534999999998</v>
+        <v>0.44192677000000002</v>
       </c>
       <c r="E37" s="2">
-        <v>0.16216958000000001</v>
+        <v>0.18890697000000001</v>
       </c>
       <c r="F37" s="2">
-        <v>0.11963037</v>
+        <v>0.12670482</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B38">
-        <v>0.28999999999999998</v>
+        <v>28.999999999999996</v>
       </c>
       <c r="C38" s="2">
-        <v>0.29106327999999998</v>
+        <v>0.19502573000000001</v>
       </c>
       <c r="D38" s="2">
-        <v>0.41593068</v>
+        <v>0.52344183</v>
       </c>
       <c r="E38" s="2">
-        <v>0.17660807000000001</v>
+        <v>0.15831734</v>
       </c>
       <c r="F38" s="2">
-        <v>0.11639797</v>
+        <v>0.12321509999999999</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B39">
-        <v>0.28999999999999998</v>
+        <v>28.999999999999996</v>
       </c>
       <c r="C39" s="2">
-        <v>0.25358749000000003</v>
+        <v>0.29106328999999997</v>
       </c>
       <c r="D39" s="2">
-        <v>0.43003052000000003</v>
+        <v>0.41593067</v>
       </c>
       <c r="E39" s="2">
-        <v>0.1885242</v>
+        <v>0.17660806000000001</v>
       </c>
       <c r="F39" s="2">
-        <v>0.12785779</v>
+        <v>0.11639797</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B40">
-        <v>0.28999999999999998</v>
+        <v>28.999999999999996</v>
       </c>
       <c r="C40" s="2">
-        <v>0.19502572000000001</v>
+        <v>0.25358749000000003</v>
       </c>
       <c r="D40" s="2">
-        <v>0.52344184000000005</v>
+        <v>0.43003052000000003</v>
       </c>
       <c r="E40" s="2">
-        <v>0.15831734</v>
+        <v>0.1885242</v>
       </c>
       <c r="F40" s="2">
-        <v>0.12321509999999999</v>
+        <v>0.12785779</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B41">
-        <v>0.31</v>
+        <v>31</v>
       </c>
       <c r="C41" s="2">
-        <v>0.30758584</v>
+        <v>0.20262593000000001</v>
       </c>
       <c r="D41" s="2">
-        <v>0.39905386999999998</v>
+        <v>0.51607702</v>
       </c>
       <c r="E41" s="2">
-        <v>0.17538173000000001</v>
+        <v>0.15446612000000001</v>
       </c>
       <c r="F41" s="2">
-        <v>0.11797856</v>
+        <v>0.12683093000000001</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B42">
-        <v>0.31</v>
+        <v>31</v>
       </c>
       <c r="C42" s="2">
-        <v>0.26498050000000001</v>
+        <v>0.30758584</v>
       </c>
       <c r="D42" s="2">
-        <v>0.41809178000000002</v>
+        <v>0.39905386999999998</v>
       </c>
       <c r="E42" s="2">
-        <v>0.18800147</v>
+        <v>0.17538173000000001</v>
       </c>
       <c r="F42" s="2">
-        <v>0.12892624999999999</v>
+        <v>0.11797856</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B43">
-        <v>0.31</v>
+        <v>31</v>
       </c>
       <c r="C43" s="2">
-        <v>0.20262593000000001</v>
+        <v>0.26498050000000001</v>
       </c>
       <c r="D43" s="2">
-        <v>0.51607702</v>
+        <v>0.41809178000000002</v>
       </c>
       <c r="E43" s="2">
-        <v>0.15446612000000001</v>
+        <v>0.18800147</v>
       </c>
       <c r="F43" s="2">
-        <v>0.12683093000000001</v>
+        <v>0.12892624999999999</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B44">
-        <v>0.33</v>
+        <v>33</v>
       </c>
       <c r="C44" s="2">
-        <v>0.32447413000000003</v>
+        <v>0.21039057</v>
       </c>
       <c r="D44" s="2">
-        <v>0.38221250000000001</v>
+        <v>0.50851698999999995</v>
       </c>
       <c r="E44" s="2">
-        <v>0.17390636000000001</v>
+        <v>0.15061902999999999</v>
       </c>
       <c r="F44" s="2">
-        <v>0.11940700999999999</v>
+        <v>0.13047341000000001</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B45">
-        <v>0.33</v>
+        <v>33</v>
       </c>
       <c r="C45" s="2">
-        <v>0.27662841999999999</v>
+        <v>0.32447411999999998</v>
       </c>
       <c r="D45" s="2">
-        <v>0.40612705999999998</v>
+        <v>0.38221252</v>
       </c>
       <c r="E45" s="2">
-        <v>0.1873379</v>
+        <v>0.17390636000000001</v>
       </c>
       <c r="F45" s="2">
-        <v>0.12990662</v>
+        <v>0.11940700999999999</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B46">
-        <v>0.33</v>
+        <v>33</v>
       </c>
       <c r="C46" s="2">
-        <v>0.21039057</v>
+        <v>0.27662840999999999</v>
       </c>
       <c r="D46" s="2">
-        <v>0.50851698999999995</v>
+        <v>0.40612706999999998</v>
       </c>
       <c r="E46" s="2">
-        <v>0.15061902999999999</v>
+        <v>0.1873379</v>
       </c>
       <c r="F46" s="2">
-        <v>0.13047341000000001</v>
+        <v>0.12990662</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B47">
-        <v>0.35</v>
+        <v>35</v>
       </c>
       <c r="C47" s="2">
-        <v>0.3416844</v>
+        <v>0.21831433</v>
       </c>
       <c r="D47" s="2">
-        <v>0.36545456999999998</v>
+        <v>0.50076852999999999</v>
       </c>
       <c r="E47" s="2">
-        <v>0.17218546000000001</v>
+        <v>0.14677924000000001</v>
       </c>
       <c r="F47" s="2">
-        <v>0.12067557</v>
+        <v>0.1341379</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B48">
-        <v>0.35</v>
+        <v>35</v>
       </c>
       <c r="C48" s="2">
-        <v>0.28851796000000002</v>
+        <v>0.3416844</v>
       </c>
       <c r="D48" s="2">
-        <v>0.39415338999999999</v>
+        <v>0.36545456999999998</v>
       </c>
       <c r="E48" s="2">
-        <v>0.18653310000000001</v>
+        <v>0.17218546000000001</v>
       </c>
       <c r="F48" s="2">
-        <v>0.13079555000000001</v>
+        <v>0.12067557</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B49">
-        <v>0.35</v>
+        <v>35</v>
       </c>
       <c r="C49" s="2">
-        <v>0.21831432000000001</v>
+        <v>0.28851796000000002</v>
       </c>
       <c r="D49" s="2">
-        <v>0.50076852999999999</v>
+        <v>0.39415338999999999</v>
       </c>
       <c r="E49" s="2">
-        <v>0.14677924000000001</v>
+        <v>0.18653310000000001</v>
       </c>
       <c r="F49" s="2">
-        <v>0.1341379</v>
+        <v>0.13079555000000001</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B50">
-        <v>0.37</v>
+        <v>37</v>
       </c>
       <c r="C50" s="2">
-        <v>0.35917027000000001</v>
+        <v>0.22639132000000001</v>
       </c>
       <c r="D50" s="2">
-        <v>0.34882797999999998</v>
+        <v>0.49283906999999999</v>
       </c>
       <c r="E50" s="2">
-        <v>0.17022428000000001</v>
+        <v>0.14295000999999999</v>
       </c>
       <c r="F50" s="2">
-        <v>0.12177746</v>
+        <v>0.13781958999999999</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B51">
-        <v>0.37</v>
+        <v>37</v>
       </c>
       <c r="C51" s="2">
-        <v>0.30063476</v>
+        <v>0.35917027000000001</v>
       </c>
       <c r="D51" s="2">
-        <v>0.38218811000000003</v>
+        <v>0.34882798999999998</v>
       </c>
       <c r="E51" s="2">
-        <v>0.18558717999999999</v>
+        <v>0.17022429</v>
       </c>
       <c r="F51" s="2">
-        <v>0.13158995000000001</v>
+        <v>0.12177746</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B52">
-        <v>0.37</v>
+        <v>37</v>
       </c>
       <c r="C52" s="2">
-        <v>0.22639133</v>
+        <v>0.30063475000000001</v>
       </c>
       <c r="D52" s="2">
-        <v>0.49283906999999999</v>
+        <v>0.38218812000000002</v>
       </c>
       <c r="E52" s="2">
-        <v>0.14295000999999999</v>
+        <v>0.18558717999999999</v>
       </c>
       <c r="F52" s="2">
-        <v>0.13781959999999999</v>
+        <v>0.13158995000000001</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B53">
-        <v>0.39</v>
+        <v>39</v>
       </c>
       <c r="C53" s="2">
-        <v>0.37688311000000002</v>
+        <v>0.23461512000000001</v>
       </c>
       <c r="D53" s="2">
-        <v>0.33238016999999997</v>
+        <v>0.48473674</v>
       </c>
       <c r="E53" s="2">
-        <v>0.16802976999999999</v>
+        <v>0.13913463000000001</v>
       </c>
       <c r="F53" s="2">
-        <v>0.12270694</v>
+        <v>0.14151351000000001</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B54">
-        <v>0.39</v>
+        <v>39</v>
       </c>
       <c r="C54" s="2">
-        <v>0.31296328000000001</v>
+        <v>0.37688312000000002</v>
       </c>
       <c r="D54" s="2">
-        <v>0.37024891999999998</v>
+        <v>0.33238015999999998</v>
       </c>
       <c r="E54" s="2">
-        <v>0.18450077000000001</v>
+        <v>0.16802976999999999</v>
       </c>
       <c r="F54" s="2">
-        <v>0.13228703</v>
+        <v>0.12270695</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B55">
-        <v>0.39</v>
+        <v>39</v>
       </c>
       <c r="C55" s="2">
-        <v>0.23461512000000001</v>
+        <v>0.31296329000000001</v>
       </c>
       <c r="D55" s="2">
-        <v>0.48473674999999999</v>
+        <v>0.37024890999999999</v>
       </c>
       <c r="E55" s="2">
-        <v>0.13913463000000001</v>
+        <v>0.18450077000000001</v>
       </c>
       <c r="F55" s="2">
-        <v>0.14151349999999999</v>
+        <v>0.13228703</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B56">
-        <v>0.41</v>
+        <v>41</v>
       </c>
       <c r="C56" s="2">
-        <v>0.39477277999999999</v>
+        <v>0.24297874</v>
       </c>
       <c r="D56" s="2">
-        <v>0.31615729999999997</v>
+        <v>0.47647028000000002</v>
       </c>
       <c r="E56" s="2">
-        <v>0.16561048</v>
+        <v>0.13533645999999999</v>
       </c>
       <c r="F56" s="2">
-        <v>0.12345943</v>
+        <v>0.14521452000000001</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B57">
-        <v>0.41</v>
+        <v>41</v>
       </c>
       <c r="C57" s="2">
-        <v>0.32548709999999997</v>
+        <v>0.39477278999999998</v>
       </c>
       <c r="D57" s="2">
-        <v>0.35835359</v>
+        <v>0.31615729999999997</v>
       </c>
       <c r="E57" s="2">
-        <v>0.18327500999999999</v>
+        <v>0.16561048</v>
       </c>
       <c r="F57" s="2">
-        <v>0.13288430000000001</v>
+        <v>0.12345943</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B58">
-        <v>0.41</v>
+        <v>41</v>
       </c>
       <c r="C58" s="2">
-        <v>0.24297874</v>
+        <v>0.32548709999999997</v>
       </c>
       <c r="D58" s="2">
-        <v>0.47647028000000002</v>
+        <v>0.35835359</v>
       </c>
       <c r="E58" s="2">
-        <v>0.13533645999999999</v>
+        <v>0.18327500999999999</v>
       </c>
       <c r="F58" s="2">
-        <v>0.14521452000000001</v>
+        <v>0.13288430000000001</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B59">
-        <v>0.43</v>
+        <v>43</v>
       </c>
       <c r="C59" s="2">
-        <v>0.41278809999999999</v>
+        <v>0.25147468000000001</v>
       </c>
       <c r="D59" s="2">
-        <v>0.30020384</v>
+        <v>0.46804905000000002</v>
       </c>
       <c r="E59" s="2">
-        <v>0.16297654</v>
+        <v>0.13155886999999999</v>
       </c>
       <c r="F59" s="2">
-        <v>0.12403152000000001</v>
+        <v>0.14891741</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B60">
-        <v>0.43</v>
+        <v>43</v>
       </c>
       <c r="C60" s="2">
-        <v>0.33818880000000001</v>
+        <v>0.41278809999999999</v>
       </c>
       <c r="D60" s="2">
-        <v>0.34651999999999999</v>
+        <v>0.30020384</v>
       </c>
       <c r="E60" s="2">
-        <v>0.18191157999999999</v>
+        <v>0.16297654</v>
       </c>
       <c r="F60" s="2">
-        <v>0.13337962</v>
+        <v>0.12403152000000001</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B61">
-        <v>0.43</v>
+        <v>43</v>
       </c>
       <c r="C61" s="2">
-        <v>0.25147468000000001</v>
+        <v>0.33818880000000001</v>
       </c>
       <c r="D61" s="2">
-        <v>0.46804905000000002</v>
+        <v>0.34651999999999999</v>
       </c>
       <c r="E61" s="2">
-        <v>0.13155886999999999</v>
+        <v>0.18191157999999999</v>
       </c>
       <c r="F61" s="2">
-        <v>0.14891741</v>
+        <v>0.13337962</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B62">
-        <v>0.45</v>
+        <v>45</v>
       </c>
       <c r="C62" s="2">
-        <v>0.43087753000000001</v>
+        <v>0.26009493</v>
       </c>
       <c r="D62" s="2">
-        <v>0.28456197999999999</v>
+        <v>0.45948302000000002</v>
       </c>
       <c r="E62" s="2">
-        <v>0.16013949999999999</v>
+        <v>0.12780523999999999</v>
       </c>
       <c r="F62" s="2">
-        <v>0.124421</v>
+        <v>0.15261680999999999</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B63">
-        <v>0.45</v>
+        <v>45</v>
       </c>
       <c r="C63" s="2">
-        <v>0.35105019999999998</v>
+        <v>0.43087754</v>
       </c>
       <c r="D63" s="2">
-        <v>0.33476593999999998</v>
+        <v>0.28456197</v>
       </c>
       <c r="E63" s="2">
-        <v>0.18041267</v>
+        <v>0.16013949</v>
       </c>
       <c r="F63" s="2">
-        <v>0.13377117999999999</v>
+        <v>0.124421</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B64">
-        <v>0.45</v>
+        <v>45</v>
       </c>
       <c r="C64" s="2">
-        <v>0.26009492000000001</v>
+        <v>0.35105020999999997</v>
       </c>
       <c r="D64" s="2">
-        <v>0.45948302000000002</v>
+        <v>0.33476593999999998</v>
       </c>
       <c r="E64" s="2">
-        <v>0.12780523999999999</v>
+        <v>0.18041267</v>
       </c>
       <c r="F64" s="2">
-        <v>0.15261680999999999</v>
+        <v>0.13377117999999999</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B65">
-        <v>0.47</v>
+        <v>47</v>
       </c>
       <c r="C65" s="2">
-        <v>0.44898983999999997</v>
+        <v>0.26883103000000003</v>
       </c>
       <c r="D65" s="2">
-        <v>0.26927107</v>
+        <v>0.45078267999999999</v>
       </c>
       <c r="E65" s="2">
-        <v>0.15711216</v>
+        <v>0.12407896</v>
       </c>
       <c r="F65" s="2">
-        <v>0.12462693</v>
+        <v>0.15630732999999999</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B66">
-        <v>0.47</v>
+        <v>47</v>
       </c>
       <c r="C66" s="2">
-        <v>0.36405248000000001</v>
+        <v>0.44898983999999997</v>
       </c>
       <c r="D66" s="2">
-        <v>0.32310897</v>
+        <v>0.26927107</v>
       </c>
       <c r="E66" s="2">
-        <v>0.17878098000000001</v>
+        <v>0.15711216</v>
       </c>
       <c r="F66" s="2">
-        <v>0.13405755999999999</v>
+        <v>0.12462693</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B67">
-        <v>0.47</v>
+        <v>47</v>
       </c>
       <c r="C67" s="2">
-        <v>0.26883103000000003</v>
+        <v>0.36405249000000001</v>
       </c>
       <c r="D67" s="2">
-        <v>0.45078267999999999</v>
+        <v>0.32310897</v>
       </c>
       <c r="E67" s="2">
-        <v>0.12407896</v>
+        <v>0.17878098000000001</v>
       </c>
       <c r="F67" s="2">
-        <v>0.15630732999999999</v>
+        <v>0.13405755999999999</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B68">
-        <v>0.49</v>
+        <v>49</v>
       </c>
       <c r="C68" s="2">
-        <v>0.46707458000000002</v>
+        <v>0.27767407999999999</v>
       </c>
       <c r="D68" s="2">
-        <v>0.25436734</v>
+        <v>0.44195904000000003</v>
       </c>
       <c r="E68" s="2">
-        <v>0.15390847999999999</v>
+        <v>0.1203834</v>
       </c>
       <c r="F68" s="2">
-        <v>0.1246496</v>
+        <v>0.15998348000000001</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B69">
-        <v>0.49</v>
+        <v>49</v>
       </c>
       <c r="C69" s="2">
-        <v>0.37717623</v>
+        <v>0.46707457000000002</v>
       </c>
       <c r="D69" s="2">
-        <v>0.31156636999999998</v>
+        <v>0.25436734</v>
       </c>
       <c r="E69" s="2">
-        <v>0.17701971999999999</v>
+        <v>0.15390847999999999</v>
       </c>
       <c r="F69" s="2">
-        <v>0.13423767</v>
+        <v>0.1246496</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B70">
-        <v>0.49</v>
+        <v>49</v>
       </c>
       <c r="C70" s="2">
-        <v>0.27767407999999999</v>
+        <v>0.37717622000000001</v>
       </c>
       <c r="D70" s="2">
-        <v>0.44195904000000003</v>
+        <v>0.31156637999999998</v>
       </c>
       <c r="E70" s="2">
-        <v>0.1203834</v>
+        <v>0.17701971999999999</v>
       </c>
       <c r="F70" s="2">
-        <v>0.15998348000000001</v>
+        <v>0.13423767</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B71">
-        <v>0.51</v>
+        <v>51</v>
       </c>
       <c r="C71" s="2">
-        <v>0.48508267999999999</v>
+        <v>0.28661477000000002</v>
       </c>
       <c r="D71" s="2">
-        <v>0.23988345</v>
+        <v>0.43302359000000001</v>
       </c>
       <c r="E71" s="2">
-        <v>0.15054338</v>
+        <v>0.11672188</v>
       </c>
       <c r="F71" s="2">
-        <v>0.12449049</v>
+        <v>0.16363976</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B72">
-        <v>0.51</v>
+        <v>51</v>
       </c>
       <c r="C72" s="2">
-        <v>0.39040156999999998</v>
+        <v>0.48508268999999998</v>
       </c>
       <c r="D72" s="2">
-        <v>0.30015499000000001</v>
+        <v>0.23988344</v>
       </c>
       <c r="E72" s="2">
-        <v>0.17513258000000001</v>
+        <v>0.15054338</v>
       </c>
       <c r="F72" s="2">
-        <v>0.13431086</v>
+        <v>0.12449049</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B73">
-        <v>0.51</v>
+        <v>51</v>
       </c>
       <c r="C73" s="2">
-        <v>0.28661476000000002</v>
+        <v>0.39040158000000003</v>
       </c>
       <c r="D73" s="2">
-        <v>0.43302360000000001</v>
+        <v>0.30015499000000001</v>
       </c>
       <c r="E73" s="2">
-        <v>0.11672188</v>
+        <v>0.17513258000000001</v>
       </c>
       <c r="F73" s="2">
-        <v>0.16363976</v>
+        <v>0.13431086</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B74">
-        <v>0.53</v>
+        <v>53</v>
       </c>
       <c r="C74" s="2">
-        <v>0.50296700999999999</v>
+        <v>0.29564342999999998</v>
       </c>
       <c r="D74" s="2">
-        <v>0.22584820999999999</v>
+        <v>0.42398823000000002</v>
       </c>
       <c r="E74" s="2">
-        <v>0.14703251000000001</v>
+        <v>0.11309768000000001</v>
       </c>
       <c r="F74" s="2">
-        <v>0.12415227</v>
+        <v>0.16727065999999999</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B75">
-        <v>0.53</v>
+        <v>53</v>
       </c>
       <c r="C75" s="2">
-        <v>0.40370837999999998</v>
+        <v>0.50296702999999998</v>
       </c>
       <c r="D75" s="2">
-        <v>0.28889110000000001</v>
+        <v>0.22584819</v>
       </c>
       <c r="E75" s="2">
-        <v>0.17312369999999999</v>
+        <v>0.14703251000000001</v>
       </c>
       <c r="F75" s="2">
-        <v>0.13427681</v>
+        <v>0.12415227</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B76">
-        <v>0.53</v>
+        <v>53</v>
       </c>
       <c r="C76" s="2">
-        <v>0.29564341999999999</v>
+        <v>0.40370840000000002</v>
       </c>
       <c r="D76" s="2">
-        <v>0.42398824000000002</v>
+        <v>0.28889109000000002</v>
       </c>
       <c r="E76" s="2">
-        <v>0.11309769</v>
+        <v>0.17312369999999999</v>
       </c>
       <c r="F76" s="2">
-        <v>0.16727065999999999</v>
+        <v>0.13427681</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B77">
-        <v>0.55000000000000004</v>
+        <v>55.000000000000007</v>
       </c>
       <c r="C77" s="2">
-        <v>0.52068278999999995</v>
+        <v>0.30475007999999998</v>
       </c>
       <c r="D77" s="2">
-        <v>0.21228638999999999</v>
+        <v>0.41486519999999999</v>
       </c>
       <c r="E77" s="2">
-        <v>0.14339210999999999</v>
+        <v>0.10951402</v>
       </c>
       <c r="F77" s="2">
-        <v>0.12363871</v>
+        <v>0.17087069999999999</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B78">
-        <v>0.55000000000000004</v>
+        <v>55.000000000000007</v>
       </c>
       <c r="C78" s="2">
-        <v>0.41707639000000002</v>
+        <v>0.52068276999999996</v>
       </c>
       <c r="D78" s="2">
-        <v>0.27779031999999998</v>
+        <v>0.21228639999999999</v>
       </c>
       <c r="E78" s="2">
-        <v>0.17099766</v>
+        <v>0.14339212000000001</v>
       </c>
       <c r="F78" s="2">
-        <v>0.13413564</v>
+        <v>0.12363871</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B79">
-        <v>0.55000000000000004</v>
+        <v>55.000000000000007</v>
       </c>
       <c r="C79" s="2">
-        <v>0.30475008999999997</v>
+        <v>0.41707638000000002</v>
       </c>
       <c r="D79" s="2">
-        <v>0.41486519999999999</v>
+        <v>0.27779031999999998</v>
       </c>
       <c r="E79" s="2">
-        <v>0.10951402</v>
+        <v>0.17099766</v>
       </c>
       <c r="F79" s="2">
-        <v>0.17087069999999999</v>
+        <v>0.13413564</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B80">
-        <v>0.56999999999999995</v>
+        <v>56.999999999999993</v>
       </c>
       <c r="C80" s="2">
-        <v>0.53818781000000004</v>
+        <v>0.31392447000000001</v>
       </c>
       <c r="D80" s="2">
-        <v>0.19921874000000001</v>
+        <v>0.4056671</v>
       </c>
       <c r="E80" s="2">
-        <v>0.13963882999999999</v>
+        <v>0.10597402</v>
       </c>
       <c r="F80" s="2">
-        <v>0.12295462</v>
+        <v>0.17443441000000001</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B81">
-        <v>0.56999999999999995</v>
+        <v>56.999999999999993</v>
       </c>
       <c r="C81" s="2">
-        <v>0.43048512999999999</v>
+        <v>0.53818781000000004</v>
       </c>
       <c r="D81" s="2">
-        <v>0.26686758999999999</v>
+        <v>0.19921874000000001</v>
       </c>
       <c r="E81" s="2">
-        <v>0.16875946</v>
+        <v>0.13963882999999999</v>
       </c>
       <c r="F81" s="2">
-        <v>0.13388783000000001</v>
+        <v>0.12295462</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B82">
-        <v>0.56999999999999995</v>
+        <v>56.999999999999993</v>
       </c>
       <c r="C82" s="2">
-        <v>0.31392447000000001</v>
+        <v>0.43048512999999999</v>
       </c>
       <c r="D82" s="2">
-        <v>0.4056671</v>
+        <v>0.26686758999999999</v>
       </c>
       <c r="E82" s="2">
-        <v>0.10597403</v>
+        <v>0.16875946</v>
       </c>
       <c r="F82" s="2">
-        <v>0.17443441000000001</v>
+        <v>0.13388783000000001</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B83">
-        <v>0.59</v>
+        <v>59</v>
       </c>
       <c r="C83" s="2">
-        <v>0.55544305000000005</v>
+        <v>0.32315611</v>
       </c>
       <c r="D83" s="2">
-        <v>0.18666173</v>
+        <v>0.39640672999999998</v>
       </c>
       <c r="E83" s="2">
-        <v>0.13578947</v>
+        <v>0.10248074</v>
       </c>
       <c r="F83" s="2">
-        <v>0.12210575</v>
+        <v>0.17795642</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B84">
-        <v>0.59</v>
+        <v>59</v>
       </c>
       <c r="C84" s="2">
-        <v>0.44391435000000001</v>
+        <v>0.55544307000000004</v>
       </c>
       <c r="D84" s="2">
-        <v>0.25613694999999997</v>
+        <v>0.18666171000000001</v>
       </c>
       <c r="E84" s="2">
-        <v>0.16641444999999999</v>
+        <v>0.13578947</v>
       </c>
       <c r="F84" s="2">
-        <v>0.13353424</v>
+        <v>0.12210575</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B85">
-        <v>0.59</v>
+        <v>59</v>
       </c>
       <c r="C85" s="2">
-        <v>0.3231561</v>
+        <v>0.44391437</v>
       </c>
       <c r="D85" s="2">
-        <v>0.39640673999999998</v>
+        <v>0.25613693999999998</v>
       </c>
       <c r="E85" s="2">
-        <v>0.10248074</v>
+        <v>0.16641444999999999</v>
       </c>
       <c r="F85" s="2">
-        <v>0.17795642</v>
+        <v>0.13353424</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B86">
-        <v>0.61</v>
+        <v>61</v>
       </c>
       <c r="C86" s="2">
-        <v>0.57241275999999996</v>
+        <v>0.33243435999999998</v>
       </c>
       <c r="D86" s="2">
-        <v>0.17462768000000001</v>
+        <v>0.38709711000000002</v>
       </c>
       <c r="E86" s="2">
-        <v>0.13186085</v>
+        <v>9.9037089999999994E-2</v>
       </c>
       <c r="F86" s="2">
-        <v>0.12109872000000001</v>
+        <v>0.18143144999999999</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B87">
-        <v>0.61</v>
+        <v>61</v>
       </c>
       <c r="C87" s="2">
-        <v>0.45734402000000002</v>
+        <v>0.57241273999999998</v>
       </c>
       <c r="D87" s="2">
-        <v>0.24561152</v>
+        <v>0.17462769</v>
       </c>
       <c r="E87" s="2">
-        <v>0.16396833999999999</v>
+        <v>0.13186085</v>
       </c>
       <c r="F87" s="2">
-        <v>0.13307611999999999</v>
+        <v>0.12109872000000001</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B88">
-        <v>0.61</v>
+        <v>61</v>
       </c>
       <c r="C88" s="2">
-        <v>0.33243435999999998</v>
+        <v>0.45734401000000002</v>
       </c>
       <c r="D88" s="2">
-        <v>0.38709710000000003</v>
+        <v>0.24561152999999999</v>
       </c>
       <c r="E88" s="2">
-        <v>9.903708E-2</v>
+        <v>0.16396833999999999</v>
       </c>
       <c r="F88" s="2">
-        <v>0.18143144999999999</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
-      <c r="F92" s="2"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
-      <c r="F95" s="2"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
-      <c r="F96" s="2"/>
-    </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
-    </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-    </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
-    </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-    </row>
-    <row r="101" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-    </row>
-    <row r="102" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
-      <c r="F102" s="2"/>
-    </row>
-    <row r="103" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-    </row>
-    <row r="104" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-    </row>
-    <row r="105" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C105" s="2"/>
-      <c r="D105" s="2"/>
-      <c r="E105" s="2"/>
-      <c r="F105" s="2"/>
-    </row>
-    <row r="106" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-      <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
-    </row>
-    <row r="107" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C107" s="2"/>
-      <c r="D107" s="2"/>
-      <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
-    </row>
-    <row r="108" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C108" s="2"/>
-      <c r="D108" s="2"/>
-      <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
-    </row>
-    <row r="109" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C109" s="2"/>
-      <c r="D109" s="2"/>
-      <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
-    </row>
-    <row r="110" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C110" s="2"/>
-      <c r="D110" s="2"/>
-      <c r="E110" s="2"/>
-      <c r="F110" s="2"/>
-    </row>
-    <row r="111" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C111" s="2"/>
-      <c r="D111" s="2"/>
-      <c r="E111" s="2"/>
-      <c r="F111" s="2"/>
-    </row>
-    <row r="112" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C112" s="2"/>
-      <c r="D112" s="2"/>
-      <c r="E112" s="2"/>
-      <c r="F112" s="2"/>
-    </row>
-    <row r="113" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C113" s="2"/>
-      <c r="D113" s="2"/>
-      <c r="E113" s="2"/>
-      <c r="F113" s="2"/>
-    </row>
-    <row r="114" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C114" s="2"/>
-      <c r="D114" s="2"/>
-      <c r="E114" s="2"/>
-      <c r="F114" s="2"/>
-    </row>
-    <row r="115" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C115" s="2"/>
-      <c r="D115" s="2"/>
-      <c r="E115" s="2"/>
-      <c r="F115" s="2"/>
-    </row>
-    <row r="116" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
-      <c r="E116" s="2"/>
-      <c r="F116" s="2"/>
-    </row>
-    <row r="117" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C117" s="2"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="2"/>
-      <c r="F117" s="2"/>
-    </row>
-    <row r="118" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C118" s="2"/>
-      <c r="D118" s="2"/>
-      <c r="E118" s="2"/>
-      <c r="F118" s="2"/>
-    </row>
-    <row r="119" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C119" s="2"/>
-      <c r="D119" s="2"/>
-      <c r="E119" s="2"/>
-      <c r="F119" s="2"/>
-    </row>
-    <row r="120" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
-      <c r="E120" s="2"/>
-      <c r="F120" s="2"/>
-    </row>
-    <row r="121" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C121" s="2"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="2"/>
-      <c r="F121" s="2"/>
-    </row>
-    <row r="122" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C122" s="2"/>
-      <c r="D122" s="2"/>
-      <c r="E122" s="2"/>
-      <c r="F122" s="2"/>
-    </row>
-    <row r="123" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
-      <c r="E123" s="2"/>
-      <c r="F123" s="2"/>
-    </row>
-    <row r="124" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C124" s="2"/>
-      <c r="D124" s="2"/>
-      <c r="E124" s="2"/>
-      <c r="F124" s="2"/>
-    </row>
-    <row r="125" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C125" s="2"/>
-      <c r="D125" s="2"/>
-      <c r="E125" s="2"/>
-      <c r="F125" s="2"/>
-    </row>
-    <row r="126" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C126" s="2"/>
-      <c r="D126" s="2"/>
-      <c r="E126" s="2"/>
-      <c r="F126" s="2"/>
-    </row>
-    <row r="127" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C127" s="2"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="2"/>
-      <c r="F127" s="2"/>
-    </row>
-    <row r="128" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C128" s="2"/>
-      <c r="D128" s="2"/>
-      <c r="E128" s="2"/>
-      <c r="F128" s="2"/>
-    </row>
-    <row r="129" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C129" s="2"/>
-      <c r="D129" s="2"/>
-      <c r="E129" s="2"/>
-      <c r="F129" s="2"/>
-    </row>
-    <row r="130" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C130" s="2"/>
-      <c r="D130" s="2"/>
-      <c r="E130" s="2"/>
-      <c r="F130" s="2"/>
-    </row>
-    <row r="131" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C131" s="2"/>
-      <c r="D131" s="2"/>
-      <c r="E131" s="2"/>
-      <c r="F131" s="2"/>
-    </row>
-    <row r="132" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C132" s="2"/>
-      <c r="D132" s="2"/>
-      <c r="E132" s="2"/>
-      <c r="F132" s="2"/>
-    </row>
-    <row r="133" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C133" s="2"/>
-      <c r="D133" s="2"/>
-      <c r="E133" s="2"/>
-      <c r="F133" s="2"/>
-    </row>
-    <row r="134" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C134" s="2"/>
-      <c r="D134" s="2"/>
-      <c r="E134" s="2"/>
-      <c r="F134" s="2"/>
-    </row>
-    <row r="135" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C135" s="2"/>
-      <c r="D135" s="2"/>
-      <c r="E135" s="2"/>
-      <c r="F135" s="2"/>
-    </row>
-    <row r="136" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C136" s="2"/>
-      <c r="D136" s="2"/>
-      <c r="E136" s="2"/>
-      <c r="F136" s="2"/>
-    </row>
-    <row r="137" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C137" s="2"/>
-      <c r="D137" s="2"/>
-      <c r="E137" s="2"/>
-      <c r="F137" s="2"/>
-    </row>
-    <row r="138" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C138" s="2"/>
-      <c r="D138" s="2"/>
-      <c r="E138" s="2"/>
-      <c r="F138" s="2"/>
-    </row>
-    <row r="139" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C139" s="2"/>
-      <c r="D139" s="2"/>
-      <c r="E139" s="2"/>
-      <c r="F139" s="2"/>
-    </row>
-    <row r="140" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C140" s="2"/>
-      <c r="D140" s="2"/>
-      <c r="E140" s="2"/>
-      <c r="F140" s="2"/>
-    </row>
-    <row r="141" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C141" s="2"/>
-      <c r="D141" s="2"/>
-      <c r="E141" s="2"/>
-      <c r="F141" s="2"/>
-    </row>
-    <row r="142" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C142" s="2"/>
-      <c r="D142" s="2"/>
-      <c r="E142" s="2"/>
-      <c r="F142" s="2"/>
-    </row>
-    <row r="143" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2"/>
-      <c r="F143" s="2"/>
-    </row>
-    <row r="144" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C144" s="2"/>
-      <c r="D144" s="2"/>
-      <c r="E144" s="2"/>
-      <c r="F144" s="2"/>
-    </row>
-    <row r="145" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C145" s="2"/>
-      <c r="D145" s="2"/>
-      <c r="E145" s="2"/>
-      <c r="F145" s="2"/>
-    </row>
-    <row r="146" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C146" s="2"/>
-      <c r="D146" s="2"/>
-      <c r="E146" s="2"/>
-      <c r="F146" s="2"/>
-    </row>
-    <row r="147" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C147" s="2"/>
-      <c r="D147" s="2"/>
-      <c r="E147" s="2"/>
-      <c r="F147" s="2"/>
-    </row>
-    <row r="148" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C148" s="2"/>
-      <c r="D148" s="2"/>
-      <c r="E148" s="2"/>
-      <c r="F148" s="2"/>
-    </row>
-    <row r="149" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C149" s="2"/>
-      <c r="D149" s="2"/>
-      <c r="E149" s="2"/>
-      <c r="F149" s="2"/>
-    </row>
-    <row r="150" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C150" s="2"/>
-      <c r="D150" s="2"/>
-      <c r="E150" s="2"/>
-      <c r="F150" s="2"/>
-    </row>
-    <row r="151" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C151" s="2"/>
-      <c r="D151" s="2"/>
-      <c r="E151" s="2"/>
-      <c r="F151" s="2"/>
-    </row>
-    <row r="152" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C152" s="2"/>
-      <c r="D152" s="2"/>
-      <c r="E152" s="2"/>
-      <c r="F152" s="2"/>
-    </row>
-    <row r="153" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C153" s="2"/>
-      <c r="D153" s="2"/>
-      <c r="E153" s="2"/>
-      <c r="F153" s="2"/>
-    </row>
-    <row r="154" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C154" s="2"/>
-      <c r="D154" s="2"/>
-      <c r="E154" s="2"/>
-      <c r="F154" s="2"/>
-    </row>
-    <row r="155" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C155" s="2"/>
-      <c r="D155" s="2"/>
-      <c r="E155" s="2"/>
-      <c r="F155" s="2"/>
-    </row>
-    <row r="156" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C156" s="2"/>
-      <c r="D156" s="2"/>
-      <c r="E156" s="2"/>
-      <c r="F156" s="2"/>
-    </row>
-    <row r="157" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C157" s="2"/>
-      <c r="D157" s="2"/>
-      <c r="E157" s="2"/>
-      <c r="F157" s="2"/>
-    </row>
-    <row r="158" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C158" s="2"/>
-      <c r="D158" s="2"/>
-      <c r="E158" s="2"/>
-      <c r="F158" s="2"/>
-    </row>
-    <row r="159" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C159" s="2"/>
-      <c r="D159" s="2"/>
-      <c r="E159" s="2"/>
-      <c r="F159" s="2"/>
-    </row>
-    <row r="160" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C160" s="2"/>
-      <c r="D160" s="2"/>
-      <c r="E160" s="2"/>
-      <c r="F160" s="2"/>
-    </row>
-    <row r="161" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C161" s="2"/>
-      <c r="D161" s="2"/>
-      <c r="E161" s="2"/>
-      <c r="F161" s="2"/>
-    </row>
-    <row r="162" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C162" s="2"/>
-      <c r="D162" s="2"/>
-      <c r="E162" s="2"/>
-      <c r="F162" s="2"/>
-    </row>
-    <row r="163" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C163" s="2"/>
-      <c r="D163" s="2"/>
-      <c r="E163" s="2"/>
-      <c r="F163" s="2"/>
-    </row>
-    <row r="164" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C164" s="2"/>
-      <c r="D164" s="2"/>
-      <c r="E164" s="2"/>
-      <c r="F164" s="2"/>
-    </row>
-    <row r="165" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C165" s="2"/>
-      <c r="D165" s="2"/>
-      <c r="E165" s="2"/>
-      <c r="F165" s="2"/>
-    </row>
-    <row r="166" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C166" s="2"/>
-      <c r="D166" s="2"/>
-      <c r="E166" s="2"/>
-      <c r="F166" s="2"/>
-    </row>
-    <row r="167" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C167" s="2"/>
-      <c r="D167" s="2"/>
-      <c r="E167" s="2"/>
-      <c r="F167" s="2"/>
-    </row>
-    <row r="168" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C168" s="2"/>
-      <c r="D168" s="2"/>
-      <c r="E168" s="2"/>
-      <c r="F168" s="2"/>
-    </row>
-    <row r="169" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C169" s="2"/>
-      <c r="D169" s="2"/>
-      <c r="E169" s="2"/>
-      <c r="F169" s="2"/>
-    </row>
-    <row r="170" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C170" s="2"/>
-      <c r="D170" s="2"/>
-      <c r="E170" s="2"/>
-      <c r="F170" s="2"/>
-    </row>
-    <row r="171" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C171" s="2"/>
-      <c r="D171" s="2"/>
-      <c r="E171" s="2"/>
-      <c r="F171" s="2"/>
-    </row>
-    <row r="172" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C172" s="2"/>
-      <c r="D172" s="2"/>
-      <c r="E172" s="2"/>
-      <c r="F172" s="2"/>
-    </row>
-    <row r="173" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C173" s="2"/>
-      <c r="D173" s="2"/>
-      <c r="E173" s="2"/>
-      <c r="F173" s="2"/>
-    </row>
-    <row r="174" spans="3:6" x14ac:dyDescent="0.45">
-      <c r="C174" s="2"/>
-      <c r="D174" s="2"/>
-      <c r="E174" s="2"/>
-      <c r="F174" s="2"/>
+        <v>0.13307611999999999</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F178">
-    <sortCondition ref="B2:B178"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F89">
+    <sortCondition ref="B2:B89"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update figures and figure data
</commit_message>
<xml_diff>
--- a/figures/fig2.xlsx
+++ b/figures/fig2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joanna\Dropbox\Repositories\ISSP_Income-Pooling\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225BDA62-99BC-4C50-8076-DEC504BE5998}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3974656B-A664-44C9-BBDC-307CCF9486EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-1860" windowWidth="30936" windowHeight="16896" xr2:uid="{8BB5332C-FFBD-4228-89AC-80112EE679CF}"/>
   </bookViews>
@@ -421,9 +421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF66AAC4-CEE8-41C4-AFD3-EB67B674149F}">
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>

</xml_diff>